<commit_message>
update firware to new version
обновил программу. исправления в платах.
</commit_message>
<xml_diff>
--- a/PCB/control_PWR_PCB/Project Outputs for control_PWR_PCB/BOM/Bill of Materials-control_PWR_PCB.xlsx
+++ b/PCB/control_PWR_PCB/Project Outputs for control_PWR_PCB/BOM/Bill of Materials-control_PWR_PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Radio\Jobe\PWR_Switch_ETH\PCB\control_PWR_PCB\Project Outputs for control_PWR_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C390BA-8CAE-42DB-B84A-83B2031F1FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4163ADE7-8539-4066-89B4-48D81ABE5056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5304" yWindow="1176" windowWidth="17280" windowHeight="10008" xr2:uid="{9C95AA7E-2B7F-4313-ACCA-F8C59F7BAD4D}"/>
+    <workbookView xWindow="3180" yWindow="0" windowWidth="17280" windowHeight="10008" xr2:uid="{99332CA1-E2CC-40FC-9343-387B9E806718}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-control_PWR_P" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
   <si>
     <t>Comment</t>
   </si>
@@ -380,16 +380,10 @@
     <t>C5, C6, C7, C8, C10, C14, C16, C18, C20, C21, C22, C24, C27, C28</t>
   </si>
   <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>Cap C</t>
   </si>
   <si>
-    <t>C2</t>
+    <t>C2, C3</t>
   </si>
   <si>
     <t>4.7 uF</t>
@@ -784,11 +778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F475FA-81A2-4B1D-A970-D7FEB8C6716F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8046758-4AA1-4844-ADF0-F4204700E970}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1536,36 +1530,24 @@
       <c r="B55" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="D55" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D56" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D57" s="4">
         <v>2</v>
       </c>
     </row>

</xml_diff>